<commit_message>
Mapping calculated values to headers
</commit_message>
<xml_diff>
--- a/ExcelReaderScript/EvaluationExcel2.xlsx
+++ b/ExcelReaderScript/EvaluationExcel2.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>MIB Resets</t>
   </si>
@@ -100,6 +100,18 @@
   </si>
   <si>
     <t>Bild Player sichtbar (USB-Android)</t>
+  </si>
+  <si>
+    <t>First result info</t>
+  </si>
+  <si>
+    <t>Second result info</t>
+  </si>
+  <si>
+    <t>Third result info</t>
+  </si>
+  <si>
+    <t>Navigation</t>
   </si>
 </sst>
 </file>
@@ -438,10 +450,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H29"/>
+  <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -582,6 +594,26 @@
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>27</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Handling for HandlePopups Output implemented
</commit_message>
<xml_diff>
--- a/ExcelReaderScript/EvaluationExcel2.xlsx
+++ b/ExcelReaderScript/EvaluationExcel2.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>MIB Resets</t>
   </si>
@@ -112,6 +112,9 @@
   </si>
   <si>
     <t>Navigation</t>
+  </si>
+  <si>
+    <t>Fourth result info</t>
   </si>
 </sst>
 </file>
@@ -450,10 +453,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H36"/>
+  <dimension ref="A1:H39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -611,8 +614,13 @@
         <v>30</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>31</v>
       </c>
     </row>

</xml_diff>